<commit_message>
Delete string resources and update file properties
</commit_message>
<xml_diff>
--- a/SignalAnalysis/localization/Russian (ru-RU) translation.xlsx
+++ b/SignalAnalysis/localization/Russian (ru-RU) translation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arthurit\source\repos\SignalAnalysis\SignalAnalysis\localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB1954D3-B94F-4925-9AB5-275055421A58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477230FD-B475-4863-970A-CA39C292821B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{611DBF29-7B42-44EF-8304-7CA1283415D8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="458">
   <si>
     <t>strAboutCompanyName</t>
   </si>
@@ -1306,31 +1306,7 @@
     <t>{0} window</t>
   </si>
   <si>
-    <t>strRadBackwardOne</t>
-  </si>
-  <si>
-    <t>Backward one-point difference</t>
-  </si>
-  <si>
-    <t>strRadCentralFive</t>
-  </si>
-  <si>
-    <t>Central five-point difference</t>
-  </si>
-  <si>
-    <t>strRadCentralThree</t>
-  </si>
-  <si>
-    <t>Central three-point difference</t>
-  </si>
-  <si>
     <t>Current culture formatting</t>
-  </si>
-  <si>
-    <t>strRadForwardOne</t>
-  </si>
-  <si>
-    <t>Forward one-point difference</t>
   </si>
   <si>
     <t>Invariant culture formatting</t>
@@ -1465,9 +1441,6 @@
   </si>
   <si>
     <t>Russian</t>
-  </si>
-  <si>
-    <t>No need, since they are already listed in strDifferentiationAlgorithms</t>
   </si>
 </sst>
 </file>
@@ -1542,8 +1515,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8A84C47E-CC65-4DC8-B540-899BE1B2B6CA}" name="Tabla1" displayName="Tabla1" ref="B2:E174" totalsRowShown="0" dataDxfId="4">
-  <autoFilter ref="B2:E174" xr:uid="{8A84C47E-CC65-4DC8-B540-899BE1B2B6CA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8A84C47E-CC65-4DC8-B540-899BE1B2B6CA}" name="Tabla1" displayName="Tabla1" ref="B2:E170" totalsRowShown="0" dataDxfId="4">
+  <autoFilter ref="B2:E170" xr:uid="{8A84C47E-CC65-4DC8-B540-899BE1B2B6CA}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{5C14670D-9FAC-4DD1-8677-28F037641DBD}" name="Key" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{E3B53744-968C-4EF6-8026-E0C57FB7D06C}" name="Comment" dataDxfId="2"/>
@@ -1851,14 +1824,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF0D1DF9-BE90-4AC9-829D-307EDF162F89}">
-  <dimension ref="B2:E174"/>
+  <dimension ref="B2:E170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.7109375" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" customWidth="1"/>
     <col min="3" max="3" width="38.5703125" customWidth="1"/>
     <col min="4" max="4" width="60.140625" customWidth="1"/>
     <col min="5" max="5" width="71.5703125" customWidth="1"/>
@@ -1869,13 +1842,13 @@
         <v>266</v>
       </c>
       <c r="C2" t="s">
-        <v>464</v>
+        <v>456</v>
       </c>
       <c r="D2" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
       <c r="E2" t="s">
-        <v>465</v>
+        <v>457</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
@@ -3416,523 +3389,475 @@
         <v>166</v>
       </c>
     </row>
-    <row r="132" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B132" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C132" s="1"/>
+      <c r="D132" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="C132" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="D132" s="1" t="s">
+      <c r="E132" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="133" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B133" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C133" s="1"/>
+      <c r="D133" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="E132" s="1"/>
-    </row>
-    <row r="133" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B133" s="1" t="s">
+      <c r="E133" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="134" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B134" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C134" s="1"/>
+      <c r="D134" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="C133" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="D133" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="E133" s="1"/>
-    </row>
-    <row r="134" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B134" s="1" t="s">
-        <v>417</v>
-      </c>
-      <c r="C134" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="D134" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="E134" s="1"/>
+      <c r="E134" s="1" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="135" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B135" s="1" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="C135" s="1"/>
       <c r="D135" s="1" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="136" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="136" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B136" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="C136" s="1" t="s">
-        <v>466</v>
-      </c>
+        <v>206</v>
+      </c>
+      <c r="C136" s="1"/>
       <c r="D136" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="E136" s="1"/>
+        <v>417</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="137" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B137" s="1" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="C137" s="1"/>
       <c r="D137" s="1" t="s">
-        <v>422</v>
+        <v>340</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="138" spans="2:5" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="138" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B138" s="1" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="C138" s="1"/>
       <c r="D138" s="1" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="139" spans="2:5" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="139" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B139" s="1" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="C139" s="1"/>
       <c r="D139" s="1" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
     </row>
     <row r="140" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B140" s="1" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="C140" s="1"/>
       <c r="D140" s="1" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
     </row>
     <row r="141" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B141" s="1" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="C141" s="1"/>
       <c r="D141" s="1" t="s">
-        <v>340</v>
+        <v>421</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="142" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="142" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B142" s="1" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="C142" s="1"/>
       <c r="D142" s="1" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="143" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="143" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B143" s="1" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="C143" s="1"/>
       <c r="D143" s="1" t="s">
-        <v>427</v>
+        <v>302</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>212</v>
+        <v>39</v>
       </c>
     </row>
     <row r="144" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B144" s="1" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="C144" s="1"/>
       <c r="D144" s="1" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="145" spans="2:5" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="145" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B145" s="1" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="C145" s="1"/>
       <c r="D145" s="1" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="146" spans="2:5" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="146" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B146" s="1" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="C146" s="1"/>
       <c r="D146" s="1" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
     </row>
     <row r="147" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B147" s="1" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="C147" s="1"/>
       <c r="D147" s="1" t="s">
-        <v>302</v>
+        <v>426</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>39</v>
+        <v>227</v>
       </c>
     </row>
     <row r="148" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B148" s="1" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="C148" s="1"/>
       <c r="D148" s="1" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="149" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="149" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B149" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="C149" s="1"/>
+        <v>428</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>430</v>
+      </c>
       <c r="D149" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="E149" s="1" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="150" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+        <v>429</v>
+      </c>
+      <c r="E149" s="1"/>
+    </row>
+    <row r="150" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B150" s="1" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="C150" s="1"/>
       <c r="D150" s="1" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
     </row>
     <row r="151" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B151" s="1" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="C151" s="1"/>
       <c r="D151" s="1" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
     </row>
     <row r="152" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B152" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="C152" s="1"/>
+        <v>433</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>430</v>
+      </c>
       <c r="D152" s="1" t="s">
-        <v>435</v>
-      </c>
-      <c r="E152" s="1" t="s">
-        <v>229</v>
-      </c>
+        <v>434</v>
+      </c>
+      <c r="E152" s="1"/>
     </row>
     <row r="153" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B153" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C153" s="1"/>
+      <c r="D153" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="E153" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="154" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B154" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="C153" s="1" t="s">
+      <c r="C154" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="D153" s="1" t="s">
+      <c r="D154" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="E153" s="1"/>
-    </row>
-    <row r="154" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B154" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="C154" s="1"/>
-      <c r="D154" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="E154" s="1" t="s">
-        <v>231</v>
-      </c>
+      <c r="E154" s="1"/>
     </row>
     <row r="155" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B155" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="C155" s="1"/>
+        <v>236</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>438</v>
+      </c>
       <c r="D155" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
     </row>
     <row r="156" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B156" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C156" s="1" t="s">
         <v>438</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E156" s="1"/>
     </row>
     <row r="157" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B157" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="C157" s="1"/>
+        <v>238</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>438</v>
+      </c>
       <c r="D157" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
     </row>
     <row r="158" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B158" s="1" t="s">
-        <v>444</v>
-      </c>
-      <c r="C158" s="1" t="s">
-        <v>446</v>
-      </c>
+        <v>240</v>
+      </c>
+      <c r="C158" s="1"/>
       <c r="D158" s="1" t="s">
-        <v>445</v>
-      </c>
-      <c r="E158" s="1"/>
+        <v>443</v>
+      </c>
+      <c r="E158" s="1" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="159" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B159" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="C159" s="1" t="s">
-        <v>446</v>
-      </c>
+        <v>242</v>
+      </c>
+      <c r="C159" s="1"/>
       <c r="D159" s="1" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
     </row>
     <row r="160" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B160" s="1" t="s">
-        <v>448</v>
-      </c>
-      <c r="C160" s="1" t="s">
-        <v>446</v>
-      </c>
+        <v>244</v>
+      </c>
+      <c r="C160" s="1"/>
       <c r="D160" s="1" t="s">
-        <v>449</v>
-      </c>
-      <c r="E160" s="1"/>
+        <v>445</v>
+      </c>
+      <c r="E160" s="1" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="161" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B161" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="C161" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C161" s="1"/>
+      <c r="D161" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="D161" s="1" t="s">
-        <v>450</v>
-      </c>
       <c r="E161" s="1" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
     </row>
     <row r="162" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B162" s="1" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="C162" s="1"/>
       <c r="D162" s="1" t="s">
-        <v>451</v>
+        <v>341</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
     </row>
     <row r="163" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B163" s="1" t="s">
-        <v>242</v>
+        <v>250</v>
       </c>
       <c r="C163" s="1"/>
       <c r="D163" s="1" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
     </row>
     <row r="164" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B164" s="1" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
       <c r="C164" s="1"/>
       <c r="D164" s="1" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>245</v>
+        <v>253</v>
       </c>
     </row>
     <row r="165" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B165" s="1" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="C165" s="1"/>
       <c r="D165" s="1" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="E165" s="1" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
     </row>
     <row r="166" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B166" s="1" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="C166" s="1"/>
       <c r="D166" s="1" t="s">
-        <v>341</v>
+        <v>450</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
     </row>
     <row r="167" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B167" s="1" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
       <c r="C167" s="1"/>
       <c r="D167" s="1" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
     </row>
     <row r="168" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B168" s="1" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
       <c r="C168" s="1"/>
       <c r="D168" s="1" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="E168" s="1" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
     </row>
     <row r="169" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B169" s="1" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="C169" s="1"/>
       <c r="D169" s="1" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="E169" s="1" t="s">
-        <v>255</v>
+        <v>263</v>
       </c>
     </row>
     <row r="170" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B170" s="1" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
       <c r="C170" s="1"/>
       <c r="D170" s="1" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="171" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B171" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="C171" s="1"/>
-      <c r="D171" s="1" t="s">
-        <v>459</v>
-      </c>
-      <c r="E171" s="1" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="172" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B172" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="C172" s="1"/>
-      <c r="D172" s="1" t="s">
-        <v>460</v>
-      </c>
-      <c r="E172" s="1" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="173" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B173" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="C173" s="1"/>
-      <c r="D173" s="1" t="s">
-        <v>461</v>
-      </c>
-      <c r="E173" s="1" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="174" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B174" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="C174" s="1"/>
-      <c r="D174" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="E174" s="1" t="s">
         <v>265</v>
       </c>
     </row>

</xml_diff>